<commit_message>
100x calibration and gain calibration
</commit_message>
<xml_diff>
--- a/beads/calc.xlsx
+++ b/beads/calc.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27105" windowHeight="11130" xr2:uid="{51A4196A-617C-44C0-B166-0DE770D241B2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27105" windowHeight="11130" activeTab="1" xr2:uid="{51A4196A-617C-44C0-B166-0DE770D241B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="polypoints" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="13">
   <si>
     <t>pixel</t>
   </si>
@@ -36,6 +37,33 @@
   </si>
   <si>
     <t>green</t>
+  </si>
+  <si>
+    <t>initial points</t>
+  </si>
+  <si>
+    <t>coef</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>coef med</t>
   </si>
 </sst>
 </file>
@@ -51,15 +79,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -67,15 +113,99 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4296,7 +4426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC2F9C7-2B8A-4BC7-8D3E-346E37D8E7E2}">
   <dimension ref="D1:AT65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC65" workbookViewId="0">
+    <sheetView topLeftCell="AC65" workbookViewId="0">
       <selection activeCell="AR62" sqref="AR62"/>
     </sheetView>
   </sheetViews>
@@ -4494,7 +4624,7 @@
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="Z3" s="2">
-        <f t="shared" ref="Z3:Z65" si="8">$Q$3*AA3^3 + $Q$4*AA3^2 + $Q$5*AA3 + $Q$6</f>
+        <f t="shared" ref="Z3:Z62" si="8">$Q$3*AA3^3 + $Q$4*AA3^2 + $Q$5*AA3 + $Q$6</f>
         <v>559.09298000000001</v>
       </c>
       <c r="AA3">
@@ -9820,7 +9950,7 @@
         <v>2391595</v>
       </c>
       <c r="AD64" s="1">
-        <f t="shared" ref="AD64:AH64" si="22">SUM(AD2:AD62)</f>
+        <f t="shared" ref="AD64:AG64" si="22">SUM(AD2:AD62)</f>
         <v>2277788</v>
       </c>
       <c r="AE64" s="1">
@@ -9884,7 +10014,7 @@
         <v>647.55892014248263</v>
       </c>
       <c r="AD65" s="3">
-        <f t="shared" ref="AD65:AH65" si="24">AD63/AD64</f>
+        <f t="shared" ref="AD65:AG65" si="24">AD63/AD64</f>
         <v>653.07444498423899</v>
       </c>
       <c r="AE65" s="3">
@@ -9946,4 +10076,876 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77594E83-AEAE-4378-88B0-EFBC6AA4FFE3}">
+  <dimension ref="C2:U41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C2" s="11"/>
+      <c r="D2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C3" s="12"/>
+      <c r="D3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C4" s="10">
+        <v>488</v>
+      </c>
+      <c r="D4" s="6">
+        <v>252</v>
+      </c>
+      <c r="E4" s="6">
+        <v>213</v>
+      </c>
+      <c r="G4" s="15">
+        <v>2.3683107199999999E-4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="10">
+        <v>488</v>
+      </c>
+      <c r="K4" s="6">
+        <v>243</v>
+      </c>
+      <c r="L4" s="6">
+        <v>227</v>
+      </c>
+      <c r="N4" s="15">
+        <v>6.5455799599999998E-4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="13">
+        <f>(G4+G11+G18+G25+G32+N4+N11+N18+N25)/9</f>
+        <v>4.6197746566666666E-4</v>
+      </c>
+      <c r="R4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="1">
+        <f>_xlfn.STDEV.P(G4,G11,G18,G25,G32,N4,N11,N18,N25)</f>
+        <v>1.829829473916334E-4</v>
+      </c>
+      <c r="U4" s="1">
+        <f>S4/Q4</f>
+        <v>0.39608630504861503</v>
+      </c>
+    </row>
+    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C5" s="4">
+        <v>592</v>
+      </c>
+      <c r="D5" s="6">
+        <v>252</v>
+      </c>
+      <c r="E5" s="6">
+        <v>255</v>
+      </c>
+      <c r="G5" s="15">
+        <v>3.7604625000000003E-2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="4">
+        <v>592</v>
+      </c>
+      <c r="K5" s="6">
+        <v>245</v>
+      </c>
+      <c r="L5" s="6">
+        <v>265</v>
+      </c>
+      <c r="N5" s="15">
+        <v>6.7290037699999999E-2</v>
+      </c>
+      <c r="O5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="14">
+        <f>(G5+G12+G19+G26+G33+N5+N12+N19+N26)/9</f>
+        <v>5.1402139744444443E-2</v>
+      </c>
+      <c r="R5" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="1">
+        <f t="shared" ref="S5:S7" si="0">_xlfn.STDEV.P(G5,G12,G19,G26,G33,N5,N12,N19,N26)</f>
+        <v>1.4509092009951667E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C6" s="4">
+        <v>680</v>
+      </c>
+      <c r="D6" s="6">
+        <v>257</v>
+      </c>
+      <c r="E6" s="6">
+        <v>283</v>
+      </c>
+      <c r="G6" s="15">
+        <v>4.2158718799999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="4">
+        <v>680</v>
+      </c>
+      <c r="K6" s="6">
+        <v>246</v>
+      </c>
+      <c r="L6" s="6">
+        <v>296</v>
+      </c>
+      <c r="N6" s="16">
+        <v>4.2387250300000003</v>
+      </c>
+      <c r="O6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="14">
+        <f t="shared" ref="Q5:Q8" si="1">(G6+G13+G20+G27+G34+N6+N13+N20+N27)/9</f>
+        <v>4.1012028733333334</v>
+      </c>
+      <c r="R6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.15179144175022913</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C7" s="4">
+        <v>735</v>
+      </c>
+      <c r="D7" s="6">
+        <v>259</v>
+      </c>
+      <c r="E7" s="6">
+        <v>296</v>
+      </c>
+      <c r="G7" s="16">
+        <v>680</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="4">
+        <v>735</v>
+      </c>
+      <c r="K7" s="6">
+        <v>248</v>
+      </c>
+      <c r="L7" s="6">
+        <v>308</v>
+      </c>
+      <c r="N7" s="16">
+        <v>680</v>
+      </c>
+      <c r="O7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="14">
+        <f t="shared" si="1"/>
+        <v>680</v>
+      </c>
+      <c r="R7" t="s">
+        <v>11</v>
+      </c>
+      <c r="S7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C9" s="11"/>
+      <c r="D9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="12"/>
+      <c r="K10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10">
+        <v>4.7898776511111119E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C11" s="10">
+        <v>488</v>
+      </c>
+      <c r="D11" s="6">
+        <f>D4+10</f>
+        <v>262</v>
+      </c>
+      <c r="E11" s="6">
+        <v>214</v>
+      </c>
+      <c r="G11" s="15">
+        <v>3.8063972E-4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="10">
+        <v>488</v>
+      </c>
+      <c r="K11" s="6">
+        <v>243</v>
+      </c>
+      <c r="L11" s="6">
+        <v>239</v>
+      </c>
+      <c r="N11" s="15">
+        <v>6.8868899500000005E-4</v>
+      </c>
+      <c r="O11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C12" s="4">
+        <v>592</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" ref="D12:D14" si="2">D5+10</f>
+        <v>262</v>
+      </c>
+      <c r="E12" s="6">
+        <v>255</v>
+      </c>
+      <c r="G12" s="15">
+        <v>4.5465020299999999E-2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="4">
+        <v>592</v>
+      </c>
+      <c r="K12" s="6">
+        <v>245</v>
+      </c>
+      <c r="L12" s="6">
+        <v>275</v>
+      </c>
+      <c r="N12" s="15">
+        <v>6.8525977500000002E-2</v>
+      </c>
+      <c r="O12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C13" s="4">
+        <v>680</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" si="2"/>
+        <v>267</v>
+      </c>
+      <c r="E13" s="6">
+        <v>283</v>
+      </c>
+      <c r="G13" s="16">
+        <v>4.1047778199999998</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="4">
+        <v>680</v>
+      </c>
+      <c r="K13" s="6">
+        <v>246</v>
+      </c>
+      <c r="L13" s="6">
+        <v>306</v>
+      </c>
+      <c r="N13" s="16">
+        <v>4.2449291899999997</v>
+      </c>
+      <c r="O13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C14" s="4">
+        <v>735</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="2"/>
+        <v>269</v>
+      </c>
+      <c r="E14" s="6">
+        <v>295</v>
+      </c>
+      <c r="G14" s="16">
+        <v>680</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="4">
+        <v>735</v>
+      </c>
+      <c r="K14" s="6">
+        <v>248</v>
+      </c>
+      <c r="L14" s="6">
+        <v>318</v>
+      </c>
+      <c r="N14" s="16">
+        <v>680</v>
+      </c>
+      <c r="O14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C16" s="11"/>
+      <c r="D16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C17" s="12"/>
+      <c r="D17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="12"/>
+      <c r="K17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C18" s="10">
+        <v>488</v>
+      </c>
+      <c r="D18" s="6">
+        <f>D11+10</f>
+        <v>272</v>
+      </c>
+      <c r="E18" s="6">
+        <v>214</v>
+      </c>
+      <c r="G18" s="15">
+        <v>3.8470004600000001E-4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="10">
+        <v>488</v>
+      </c>
+      <c r="K18" s="6">
+        <v>243</v>
+      </c>
+      <c r="L18" s="6">
+        <v>250</v>
+      </c>
+      <c r="N18" s="15">
+        <v>6.8443142100000005E-4</v>
+      </c>
+      <c r="O18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C19" s="4">
+        <v>592</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" ref="D19:D21" si="3">D12+10</f>
+        <v>272</v>
+      </c>
+      <c r="E19" s="6">
+        <v>255</v>
+      </c>
+      <c r="G19" s="15">
+        <v>4.5216599500000003E-2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="4">
+        <v>592</v>
+      </c>
+      <c r="K19" s="6">
+        <v>245</v>
+      </c>
+      <c r="L19" s="6">
+        <v>289</v>
+      </c>
+      <c r="N19" s="15">
+        <v>7.1511748599999994E-2</v>
+      </c>
+      <c r="O19" t="s">
+        <v>9</v>
+      </c>
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C20" s="4">
+        <v>680</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" si="3"/>
+        <v>277</v>
+      </c>
+      <c r="E20" s="6">
+        <v>283</v>
+      </c>
+      <c r="G20" s="16">
+        <v>4.0867856500000004</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="4">
+        <v>680</v>
+      </c>
+      <c r="K20" s="6">
+        <v>246</v>
+      </c>
+      <c r="L20" s="6">
+        <v>321</v>
+      </c>
+      <c r="N20" s="15">
+        <v>4.29332358</v>
+      </c>
+      <c r="O20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C21" s="4">
+        <v>735</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="3"/>
+        <v>279</v>
+      </c>
+      <c r="E21" s="6">
+        <v>295</v>
+      </c>
+      <c r="G21" s="16">
+        <v>680</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="4">
+        <v>735</v>
+      </c>
+      <c r="K21" s="6">
+        <v>248</v>
+      </c>
+      <c r="L21" s="6">
+        <v>333</v>
+      </c>
+      <c r="N21" s="16">
+        <v>680</v>
+      </c>
+      <c r="O21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C23" s="11"/>
+      <c r="D23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C24" s="12"/>
+      <c r="D24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C25" s="10">
+        <v>488</v>
+      </c>
+      <c r="D25" s="6">
+        <v>275</v>
+      </c>
+      <c r="E25" s="6">
+        <v>214</v>
+      </c>
+      <c r="G25" s="15">
+        <v>2.7190682899999998E-4</v>
+      </c>
+      <c r="H25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="10">
+        <v>488</v>
+      </c>
+      <c r="K25" s="6">
+        <v>243</v>
+      </c>
+      <c r="L25" s="6">
+        <v>263</v>
+      </c>
+      <c r="N25" s="15">
+        <v>6.0360838800000002E-4</v>
+      </c>
+      <c r="O25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C26" s="4">
+        <v>592</v>
+      </c>
+      <c r="D26" s="6">
+        <v>278</v>
+      </c>
+      <c r="E26" s="6">
+        <v>255</v>
+      </c>
+      <c r="G26" s="15">
+        <v>3.47540551E-2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="4">
+        <v>592</v>
+      </c>
+      <c r="K26" s="6">
+        <v>245</v>
+      </c>
+      <c r="L26" s="6">
+        <v>300</v>
+      </c>
+      <c r="N26" s="15">
+        <v>5.9313698300000002E-2</v>
+      </c>
+      <c r="O26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C27" s="4">
+        <v>680</v>
+      </c>
+      <c r="D27" s="6">
+        <v>280</v>
+      </c>
+      <c r="E27" s="6">
+        <v>283</v>
+      </c>
+      <c r="G27" s="16">
+        <v>3.8993954500000001</v>
+      </c>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="4">
+        <v>680</v>
+      </c>
+      <c r="K27" s="6">
+        <v>246</v>
+      </c>
+      <c r="L27" s="6">
+        <v>332</v>
+      </c>
+      <c r="N27" s="15">
+        <v>3.9697745200000001</v>
+      </c>
+      <c r="O27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C28" s="4">
+        <v>735</v>
+      </c>
+      <c r="D28" s="6">
+        <v>280</v>
+      </c>
+      <c r="E28" s="6">
+        <v>295</v>
+      </c>
+      <c r="G28" s="16">
+        <v>680</v>
+      </c>
+      <c r="H28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" s="4">
+        <v>735</v>
+      </c>
+      <c r="K28" s="6">
+        <v>248</v>
+      </c>
+      <c r="L28" s="6">
+        <v>345</v>
+      </c>
+      <c r="N28" s="16">
+        <v>680</v>
+      </c>
+      <c r="O28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C30" s="11"/>
+      <c r="D30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C31" s="12"/>
+      <c r="D31" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C32" s="10">
+        <v>488</v>
+      </c>
+      <c r="D32" s="6">
+        <f>D25+10</f>
+        <v>285</v>
+      </c>
+      <c r="E32" s="6">
+        <v>214</v>
+      </c>
+      <c r="G32" s="15">
+        <v>2.5243272400000001E-4</v>
+      </c>
+      <c r="H32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C33" s="4">
+        <v>592</v>
+      </c>
+      <c r="D33" s="6">
+        <f t="shared" ref="D33:D35" si="4">D26+10</f>
+        <v>288</v>
+      </c>
+      <c r="E33" s="6">
+        <v>255</v>
+      </c>
+      <c r="G33" s="15">
+        <v>3.29374957E-2</v>
+      </c>
+      <c r="H33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C34" s="4">
+        <v>680</v>
+      </c>
+      <c r="D34" s="6">
+        <f t="shared" si="4"/>
+        <v>290</v>
+      </c>
+      <c r="E34" s="6">
+        <v>283</v>
+      </c>
+      <c r="G34" s="16">
+        <v>3.8572427399999998</v>
+      </c>
+      <c r="H34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C35" s="4">
+        <v>735</v>
+      </c>
+      <c r="D35" s="6">
+        <f t="shared" si="4"/>
+        <v>290</v>
+      </c>
+      <c r="E35" s="6">
+        <v>295</v>
+      </c>
+      <c r="G35" s="16">
+        <v>680</v>
+      </c>
+      <c r="H35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="G37" s="1">
+        <f>AVERAGE(G4,G25,G32)</f>
+        <v>2.5372354166666662E-4</v>
+      </c>
+      <c r="N37" s="1">
+        <f>AVERAGE(N4,N11,N18,N25)</f>
+        <v>6.5782170000000008E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="G38" s="1">
+        <f t="shared" ref="G38:G39" si="5">AVERAGE(G5,G26,G33)</f>
+        <v>3.5098725266666665E-2</v>
+      </c>
+      <c r="N38" s="1">
+        <f t="shared" ref="N38:N40" si="6">AVERAGE(N5,N12,N19,N26)</f>
+        <v>6.6660365525000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="G39" s="1">
+        <f t="shared" si="5"/>
+        <v>3.9908366900000001</v>
+      </c>
+      <c r="N39" s="1">
+        <f t="shared" si="6"/>
+        <v>4.1866880800000006</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="G40" s="1">
+        <f t="shared" ref="G38:G40" si="7">AVERAGE(G7,G14,G21,G28,G35)</f>
+        <v>680</v>
+      </c>
+      <c r="N40" s="1">
+        <f t="shared" si="6"/>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="G41" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D23:E23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>